<commit_message>
updated VerifPlan with information regarding code coverage
</commit_message>
<xml_diff>
--- a/docs/VerifPlan.xlsx
+++ b/docs/VerifPlan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -88,6 +88,29 @@
   </si>
   <si>
     <t>Valid signal for the output bus must be asserted on the next cycle of of valid signal for the input domain</t>
+  </si>
+  <si>
+    <t>https://github.com/npatsiatzis/simple_adder/blob/main/uvm_sim/sbm_cov.txt</t>
+  </si>
+  <si>
+    <t>o_C &lt; ((2**(g_data_width+1)) -1)</t>
+  </si>
+  <si>
+    <t>The addition output is between its specified range of values</t>
+  </si>
+  <si>
+    <r>
+      <t>*Code Coverage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (statement, branch, FSM, assertion) can be found in : https://github.com/npatsiatzis/simple_adder/blob/main/uvm_sim/sbm_cov.txt</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve"> -------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------- END -----------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------</t>
@@ -134,12 +157,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -162,6 +185,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="DejaVu Sans"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="DejaVu Sans"/>
       <charset val="1"/>
@@ -180,6 +210,66 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -189,7 +279,53 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -210,118 +346,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -338,181 +368,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -532,11 +562,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -573,8 +618,10 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -595,32 +642,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -629,145 +650,154 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -790,8 +820,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="48" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="48" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1184,16 +1217,16 @@
   <sheetPr/>
   <dimension ref="A1:I84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.0074074074074" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="21.2888888888889" style="5" customWidth="1"/>
-    <col min="2" max="2" width="20.2962962962963" style="5" customWidth="1"/>
+    <col min="2" max="2" width="24.1703703703704" style="5" customWidth="1"/>
     <col min="3" max="3" width="12.1407407407407" style="5" customWidth="1"/>
     <col min="4" max="4" width="51.2888888888889" style="5" customWidth="1"/>
     <col min="5" max="5" width="41.2888888888889" style="5" customWidth="1"/>
@@ -1227,10 +1260,10 @@
       <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1257,7 +1290,7 @@
       <c r="H2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="12" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1282,7 +1315,7 @@
       <c r="H3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="12" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1307,30 +1340,45 @@
       <c r="H4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" s="3" customFormat="1" spans="1:9">
+      <c r="I4" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" s="3" customFormat="1" ht="42.75" spans="1:9">
       <c r="A5" s="8"/>
       <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
+      <c r="C5" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="6" s="3" customFormat="1" spans="1:9">
       <c r="A6" s="8"/>
       <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
+      <c r="I6" s="12"/>
     </row>
     <row r="7" s="3" customFormat="1" spans="1:9">
       <c r="A7" s="8"/>
@@ -1362,9 +1410,11 @@
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
     </row>
-    <row r="10" s="3" customFormat="1" spans="1:9">
+    <row r="10" s="3" customFormat="1" ht="87" spans="1:9">
       <c r="A10" s="8"/>
-      <c r="B10" s="9"/>
+      <c r="B10" s="10" t="s">
+        <v>27</v>
+      </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
@@ -2163,37 +2213,38 @@
       <c r="I83" s="8"/>
     </row>
     <row r="84" s="4" customFormat="1" spans="1:9">
-      <c r="A84" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B84" s="12"/>
-      <c r="C84" s="12"/>
-      <c r="D84" s="12"/>
-      <c r="E84" s="12"/>
-      <c r="F84" s="12"/>
-      <c r="G84" s="12"/>
-      <c r="H84" s="12"/>
-      <c r="I84" s="12"/>
+      <c r="A84" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B84" s="13"/>
+      <c r="C84" s="13"/>
+      <c r="D84" s="13"/>
+      <c r="E84" s="13"/>
+      <c r="F84" s="13"/>
+      <c r="G84" s="13"/>
+      <c r="H84" s="13"/>
+      <c r="I84" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A84:I84"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G83">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G3 G4:G6 G7:G83">
       <formula1>DONOTDELETE!$C$3:$C$10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H83">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H3 H4:H6 H7:H83">
       <formula1>DONOTDELETE!$E$3:$E$7</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F83">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F3 F4:F6 F7:F83">
       <formula1>DONOTDELETE!$A$3:$A$10</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" display="https://github.com/npatsiatzis/simple_adder/blob/main/pyuvm_sim/coverage_pyuvm.xml"/>
     <hyperlink ref="I3" r:id="rId1" display="https://github.com/npatsiatzis/simple_adder/blob/main/pyuvm_sim/coverage_pyuvm.xml"/>
-    <hyperlink ref="I4" r:id="rId1" display="https://github.com/npatsiatzis/simple_adder/blob/main/pyuvm_sim/coverage_pyuvm.xml"/>
+    <hyperlink ref="I4" r:id="rId2" display="https://github.com/npatsiatzis/simple_adder/blob/main/uvm_sim/sbm_cov.txt" tooltip="https://github.com/npatsiatzis/simple_adder/blob/main/uvm_sim/sbm_cov.txt"/>
+    <hyperlink ref="I5" r:id="rId2" display="https://github.com/npatsiatzis/simple_adder/blob/main/uvm_sim/sbm_cov.txt" tooltip="https://github.com/npatsiatzis/simple_adder/blob/main/uvm_sim/sbm_cov.txt"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -2235,18 +2286,18 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
@@ -2254,10 +2305,10 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
         <v>21</v>
@@ -2268,42 +2319,42 @@
         <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="3:3">
       <c r="C10" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>